<commit_message>
test cases for new features in dba
</commit_message>
<xml_diff>
--- a/Norvic International Hospital/Documents/Test cases NIH BackEnd.xlsx
+++ b/Norvic International Hospital/Documents/Test cases NIH BackEnd.xlsx
@@ -16,6 +16,7 @@
     <sheet name="Feedback Management" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -370,12 +371,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -383,6 +378,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -718,7 +719,7 @@
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="A3" s="12">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -746,7 +747,7 @@
       <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5"/>
@@ -780,7 +781,7 @@
       <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="12">
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -810,7 +811,7 @@
       <c r="L6" s="3"/>
     </row>
     <row r="7" spans="1:12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
       <c r="D7" s="5"/>
@@ -844,7 +845,7 @@
       <c r="L8" s="3"/>
     </row>
     <row r="9" spans="1:12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="A9" s="12">
         <v>3</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -872,7 +873,7 @@
       <c r="L9" s="3"/>
     </row>
     <row r="10" spans="1:12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
       <c r="D10" s="5"/>
@@ -892,7 +893,7 @@
       <c r="L10" s="3"/>
     </row>
     <row r="11" spans="1:12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="5"/>
       <c r="C11" s="6"/>
       <c r="D11" s="5"/>
@@ -912,7 +913,7 @@
       <c r="L11" s="3"/>
     </row>
     <row r="12" spans="1:12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="5"/>
       <c r="C12" s="6"/>
       <c r="D12" s="5"/>
@@ -932,7 +933,7 @@
       <c r="L12" s="3"/>
     </row>
     <row r="13" spans="1:12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
       <c r="D13" s="5"/>
@@ -952,7 +953,7 @@
       <c r="L13" s="3"/>
     </row>
     <row r="14" spans="1:12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
       <c r="D14" s="5"/>
@@ -972,7 +973,7 @@
       <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
       <c r="D15" s="5"/>
@@ -992,7 +993,7 @@
       <c r="L15" s="3"/>
     </row>
     <row r="16" spans="1:12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="5"/>
       <c r="C16" s="6"/>
       <c r="D16" s="5"/>
@@ -1012,7 +1013,7 @@
       <c r="L16" s="3"/>
     </row>
     <row r="17" spans="1:12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="5"/>
       <c r="C17" s="6"/>
       <c r="D17" s="5"/>
@@ -1032,7 +1033,7 @@
       <c r="L17" s="3"/>
     </row>
     <row r="18" spans="1:12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="5"/>
       <c r="C18" s="6"/>
       <c r="D18" s="5"/>
@@ -1066,7 +1067,7 @@
       <c r="L19" s="3"/>
     </row>
     <row r="20" spans="1:12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
+      <c r="A20" s="12">
         <v>3</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -1094,7 +1095,7 @@
       <c r="L20" s="3"/>
     </row>
     <row r="21" spans="1:12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="5"/>
       <c r="C21" s="6"/>
       <c r="D21" s="5"/>
@@ -1114,7 +1115,7 @@
       <c r="L21" s="3"/>
     </row>
     <row r="22" spans="1:12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="5"/>
       <c r="C22" s="6"/>
       <c r="D22" s="5"/>
@@ -1148,7 +1149,7 @@
       <c r="L23" s="3"/>
     </row>
     <row r="24" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
+      <c r="A24" s="11">
         <v>4</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -1174,7 +1175,7 @@
       <c r="J24" s="7"/>
     </row>
     <row r="25" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
+      <c r="A25" s="11"/>
       <c r="C25" s="6"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7">
@@ -1191,7 +1192,7 @@
       <c r="J25" s="7"/>
     </row>
     <row r="26" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
+      <c r="A26" s="11"/>
       <c r="C26" s="6"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7">
@@ -1208,7 +1209,7 @@
       <c r="J26" s="7"/>
     </row>
     <row r="27" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
+      <c r="A27" s="11"/>
       <c r="C27" s="6"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7">
@@ -1236,7 +1237,7 @@
       <c r="J28" s="7"/>
     </row>
     <row r="29" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
+      <c r="A29" s="11">
         <v>5</v>
       </c>
       <c r="B29" s="7" t="s">
@@ -1262,7 +1263,7 @@
       <c r="J29" s="7"/>
     </row>
     <row r="30" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
+      <c r="A30" s="11"/>
       <c r="C30" s="6"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7">
@@ -1279,7 +1280,7 @@
       <c r="J30" s="7"/>
     </row>
     <row r="31" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
+      <c r="A31" s="11"/>
       <c r="C31" s="6"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7">
@@ -4393,12 +4394,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A29:A31"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A9:A18"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A29:A31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4415,7 +4416,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="12"/>
+    <col min="1" max="1" width="9.140625" style="10"/>
     <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="3" width="28.140625" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
@@ -4458,7 +4459,7 @@
       <c r="A2"/>
     </row>
     <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
+      <c r="A3" s="8">
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -4483,7 +4484,7 @@
       <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -4500,7 +4501,7 @@
       <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -4511,7 +4512,7 @@
       <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+      <c r="A6" s="8">
         <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -4536,7 +4537,7 @@
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -4553,7 +4554,7 @@
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -4570,7 +4571,7 @@
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -4581,7 +4582,7 @@
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+      <c r="A10" s="8">
         <v>3</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -4604,7 +4605,7 @@
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -4621,7 +4622,7 @@
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -4636,7 +4637,7 @@
       <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -4655,7 +4656,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -4666,7 +4667,7 @@
       <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
+      <c r="A15" s="8">
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
@@ -4681,7 +4682,7 @@
       <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -4692,7 +4693,7 @@
       <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
+      <c r="A17" s="8"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -4703,7 +4704,7 @@
       <c r="I17" s="6"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
+      <c r="A18" s="8"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -4714,7 +4715,7 @@
       <c r="I18" s="6"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
+      <c r="A19" s="8"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
@@ -4725,7 +4726,7 @@
       <c r="I19" s="6"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
+      <c r="A20" s="8"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
@@ -4736,7 +4737,7 @@
       <c r="I20" s="6"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
+      <c r="A21" s="8"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
@@ -4747,7 +4748,7 @@
       <c r="I21" s="6"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
+      <c r="A22" s="8"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -4758,7 +4759,7 @@
       <c r="I22" s="6"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
+      <c r="A23" s="8"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -4769,7 +4770,7 @@
       <c r="I23" s="6"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
+      <c r="A24" s="8"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -4780,7 +4781,7 @@
       <c r="I24" s="6"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
+      <c r="A25" s="8"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -4791,7 +4792,7 @@
       <c r="I25" s="6"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
+      <c r="A26" s="8"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -4802,7 +4803,7 @@
       <c r="I26" s="6"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
+      <c r="A27" s="8"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -4813,7 +4814,7 @@
       <c r="I27" s="6"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
+      <c r="A28" s="8"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -4824,7 +4825,7 @@
       <c r="I28" s="6"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
+      <c r="A29" s="8"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
@@ -4835,7 +4836,7 @@
       <c r="I29" s="6"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
+      <c r="A30" s="8"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
@@ -4846,7 +4847,7 @@
       <c r="I30" s="6"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
+      <c r="A31" s="8"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
@@ -4857,7 +4858,7 @@
       <c r="I31" s="6"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
+      <c r="A32" s="8"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
@@ -4868,7 +4869,7 @@
       <c r="I32" s="6"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
+      <c r="A33" s="8"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
@@ -4879,7 +4880,7 @@
       <c r="I33" s="6"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
+      <c r="A34" s="8"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
@@ -4890,7 +4891,7 @@
       <c r="I34" s="6"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="10"/>
+      <c r="A35" s="8"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
@@ -4901,7 +4902,7 @@
       <c r="I35" s="6"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="10"/>
+      <c r="A36" s="8"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
@@ -4912,7 +4913,7 @@
       <c r="I36" s="6"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="10"/>
+      <c r="A37" s="8"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
@@ -4923,7 +4924,7 @@
       <c r="I37" s="6"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="10"/>
+      <c r="A38" s="8"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
@@ -4934,7 +4935,7 @@
       <c r="I38" s="6"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="10"/>
+      <c r="A39" s="8"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
@@ -4945,7 +4946,7 @@
       <c r="I39" s="6"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="10"/>
+      <c r="A40" s="8"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
@@ -4956,7 +4957,7 @@
       <c r="I40" s="6"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="10"/>
+      <c r="A41" s="8"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
@@ -4967,7 +4968,7 @@
       <c r="I41" s="6"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="10"/>
+      <c r="A42" s="8"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
@@ -4978,7 +4979,7 @@
       <c r="I42" s="6"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="10"/>
+      <c r="A43" s="8"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
@@ -4989,7 +4990,7 @@
       <c r="I43" s="6"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="10"/>
+      <c r="A44" s="8"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
@@ -5000,7 +5001,7 @@
       <c r="I44" s="6"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="10"/>
+      <c r="A45" s="8"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
@@ -5011,7 +5012,7 @@
       <c r="I45" s="6"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="10"/>
+      <c r="A46" s="8"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
@@ -5022,7 +5023,7 @@
       <c r="I46" s="6"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="10"/>
+      <c r="A47" s="8"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
@@ -5033,7 +5034,7 @@
       <c r="I47" s="6"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="10"/>
+      <c r="A48" s="8"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
@@ -5044,7 +5045,7 @@
       <c r="I48" s="6"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="10"/>
+      <c r="A49" s="8"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
@@ -5055,7 +5056,7 @@
       <c r="I49" s="6"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="10"/>
+      <c r="A50" s="8"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
@@ -5066,7 +5067,7 @@
       <c r="I50" s="6"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="10"/>
+      <c r="A51" s="8"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
@@ -5077,7 +5078,7 @@
       <c r="I51" s="6"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="10"/>
+      <c r="A52" s="8"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
@@ -5088,7 +5089,7 @@
       <c r="I52" s="6"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="10"/>
+      <c r="A53" s="8"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
@@ -5099,7 +5100,7 @@
       <c r="I53" s="6"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="10"/>
+      <c r="A54" s="8"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
@@ -5110,7 +5111,7 @@
       <c r="I54" s="6"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="10"/>
+      <c r="A55" s="8"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
@@ -5121,7 +5122,7 @@
       <c r="I55" s="6"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="10"/>
+      <c r="A56" s="8"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
@@ -5132,7 +5133,7 @@
       <c r="I56" s="6"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="10"/>
+      <c r="A57" s="8"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
@@ -5143,7 +5144,7 @@
       <c r="I57" s="6"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="10"/>
+      <c r="A58" s="8"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
@@ -5154,7 +5155,7 @@
       <c r="I58" s="6"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="10"/>
+      <c r="A59" s="8"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
@@ -5165,7 +5166,7 @@
       <c r="I59" s="6"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="10"/>
+      <c r="A60" s="8"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
@@ -5176,7 +5177,7 @@
       <c r="I60" s="6"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="10"/>
+      <c r="A61" s="8"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
@@ -5187,7 +5188,7 @@
       <c r="I61" s="6"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="10"/>
+      <c r="A62" s="8"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
       <c r="D62" s="6"/>
@@ -5198,7 +5199,7 @@
       <c r="I62" s="6"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="10"/>
+      <c r="A63" s="8"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
       <c r="D63" s="6"/>
@@ -5209,7 +5210,7 @@
       <c r="I63" s="6"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="10"/>
+      <c r="A64" s="8"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
       <c r="D64" s="6"/>
@@ -5220,7 +5221,7 @@
       <c r="I64" s="6"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="10"/>
+      <c r="A65" s="8"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
       <c r="D65" s="6"/>
@@ -5231,7 +5232,7 @@
       <c r="I65" s="6"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="10"/>
+      <c r="A66" s="8"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
       <c r="D66" s="6"/>
@@ -5242,7 +5243,7 @@
       <c r="I66" s="6"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="10"/>
+      <c r="A67" s="8"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
       <c r="D67" s="6"/>
@@ -5253,7 +5254,7 @@
       <c r="I67" s="6"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="10"/>
+      <c r="A68" s="8"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
       <c r="D68" s="6"/>
@@ -5264,7 +5265,7 @@
       <c r="I68" s="6"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="10"/>
+      <c r="A69" s="8"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
       <c r="D69" s="6"/>
@@ -5275,7 +5276,7 @@
       <c r="I69" s="6"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="10"/>
+      <c r="A70" s="8"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
       <c r="D70" s="6"/>
@@ -5286,7 +5287,7 @@
       <c r="I70" s="6"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="10"/>
+      <c r="A71" s="8"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
       <c r="D71" s="6"/>
@@ -5297,7 +5298,7 @@
       <c r="I71" s="6"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="10"/>
+      <c r="A72" s="8"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
       <c r="D72" s="6"/>
@@ -5308,7 +5309,7 @@
       <c r="I72" s="6"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="10"/>
+      <c r="A73" s="8"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
       <c r="D73" s="6"/>
@@ -5319,7 +5320,7 @@
       <c r="I73" s="6"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="10"/>
+      <c r="A74" s="8"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
       <c r="D74" s="6"/>
@@ -5330,7 +5331,7 @@
       <c r="I74" s="6"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="10"/>
+      <c r="A75" s="8"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
       <c r="D75" s="6"/>
@@ -5341,7 +5342,7 @@
       <c r="I75" s="6"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="10"/>
+      <c r="A76" s="8"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
       <c r="D76" s="6"/>
@@ -5352,7 +5353,7 @@
       <c r="I76" s="6"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="10"/>
+      <c r="A77" s="8"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
       <c r="D77" s="6"/>
@@ -5363,7 +5364,7 @@
       <c r="I77" s="6"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="10"/>
+      <c r="A78" s="8"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
@@ -5374,7 +5375,7 @@
       <c r="I78" s="6"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="10"/>
+      <c r="A79" s="8"/>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
       <c r="D79" s="6"/>
@@ -5385,7 +5386,7 @@
       <c r="I79" s="6"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="10"/>
+      <c r="A80" s="8"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
       <c r="D80" s="6"/>
@@ -5396,7 +5397,7 @@
       <c r="I80" s="6"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="10"/>
+      <c r="A81" s="8"/>
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
       <c r="D81" s="6"/>
@@ -5407,7 +5408,7 @@
       <c r="I81" s="6"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" s="10"/>
+      <c r="A82" s="8"/>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
       <c r="D82" s="6"/>
@@ -5418,7 +5419,7 @@
       <c r="I82" s="6"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="10"/>
+      <c r="A83" s="8"/>
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
       <c r="D83" s="6"/>
@@ -5429,7 +5430,7 @@
       <c r="I83" s="6"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="10"/>
+      <c r="A84" s="8"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
       <c r="D84" s="6"/>
@@ -5440,7 +5441,7 @@
       <c r="I84" s="6"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="10"/>
+      <c r="A85" s="8"/>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
       <c r="D85" s="6"/>
@@ -5451,7 +5452,7 @@
       <c r="I85" s="6"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A86" s="10"/>
+      <c r="A86" s="8"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
       <c r="D86" s="6"/>
@@ -5462,7 +5463,7 @@
       <c r="I86" s="6"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" s="10"/>
+      <c r="A87" s="8"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
       <c r="D87" s="6"/>
@@ -5473,7 +5474,7 @@
       <c r="I87" s="6"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A88" s="10"/>
+      <c r="A88" s="8"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
       <c r="D88" s="6"/>
@@ -5484,7 +5485,7 @@
       <c r="I88" s="6"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" s="10"/>
+      <c r="A89" s="8"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
       <c r="D89" s="6"/>
@@ -5495,7 +5496,7 @@
       <c r="I89" s="6"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A90" s="10"/>
+      <c r="A90" s="8"/>
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
       <c r="D90" s="6"/>
@@ -5506,7 +5507,7 @@
       <c r="I90" s="6"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A91" s="10"/>
+      <c r="A91" s="8"/>
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
       <c r="D91" s="6"/>
@@ -5517,7 +5518,7 @@
       <c r="I91" s="6"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A92" s="10"/>
+      <c r="A92" s="8"/>
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
       <c r="D92" s="6"/>
@@ -5528,7 +5529,7 @@
       <c r="I92" s="6"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A93" s="10"/>
+      <c r="A93" s="8"/>
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
       <c r="D93" s="6"/>
@@ -5539,7 +5540,7 @@
       <c r="I93" s="6"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" s="10"/>
+      <c r="A94" s="8"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
       <c r="D94" s="6"/>
@@ -5550,7 +5551,7 @@
       <c r="I94" s="6"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A95" s="10"/>
+      <c r="A95" s="8"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
       <c r="D95" s="6"/>
@@ -5561,7 +5562,7 @@
       <c r="I95" s="6"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96" s="10"/>
+      <c r="A96" s="8"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
       <c r="D96" s="6"/>
@@ -5572,7 +5573,7 @@
       <c r="I96" s="6"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" s="10"/>
+      <c r="A97" s="8"/>
       <c r="B97" s="6"/>
       <c r="C97" s="6"/>
       <c r="D97" s="6"/>
@@ -5583,7 +5584,7 @@
       <c r="I97" s="6"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A98" s="11"/>
+      <c r="A98" s="9"/>
       <c r="B98" s="6"/>
       <c r="C98" s="6"/>
       <c r="D98" s="3"/>
@@ -5594,7 +5595,7 @@
       <c r="I98" s="3"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A99" s="11"/>
+      <c r="A99" s="9"/>
       <c r="B99" s="6"/>
       <c r="C99" s="6"/>
       <c r="D99" s="3"/>
@@ -5605,7 +5606,7 @@
       <c r="I99" s="3"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A100" s="11"/>
+      <c r="A100" s="9"/>
       <c r="B100" s="6"/>
       <c r="C100" s="6"/>
       <c r="D100" s="3"/>
@@ -5616,7 +5617,7 @@
       <c r="I100" s="3"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="11"/>
+      <c r="A101" s="9"/>
       <c r="B101" s="6"/>
       <c r="C101" s="6"/>
       <c r="D101" s="3"/>
@@ -5627,7 +5628,7 @@
       <c r="I101" s="3"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A102" s="11"/>
+      <c r="A102" s="9"/>
       <c r="B102" s="6"/>
       <c r="C102" s="6"/>
       <c r="D102" s="3"/>
@@ -5638,7 +5639,7 @@
       <c r="I102" s="3"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="11"/>
+      <c r="A103" s="9"/>
       <c r="B103" s="6"/>
       <c r="C103" s="6"/>
       <c r="D103" s="3"/>
@@ -5649,7 +5650,7 @@
       <c r="I103" s="3"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="11"/>
+      <c r="A104" s="9"/>
       <c r="B104" s="6"/>
       <c r="C104" s="6"/>
       <c r="D104" s="3"/>
@@ -5660,7 +5661,7 @@
       <c r="I104" s="3"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105" s="11"/>
+      <c r="A105" s="9"/>
       <c r="B105" s="6"/>
       <c r="C105" s="6"/>
       <c r="D105" s="3"/>
@@ -5671,7 +5672,7 @@
       <c r="I105" s="3"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106" s="11"/>
+      <c r="A106" s="9"/>
       <c r="B106" s="6"/>
       <c r="C106" s="6"/>
       <c r="D106" s="3"/>
@@ -5682,7 +5683,7 @@
       <c r="I106" s="3"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" s="11"/>
+      <c r="A107" s="9"/>
       <c r="B107" s="6"/>
       <c r="C107" s="6"/>
       <c r="D107" s="3"/>
@@ -5693,7 +5694,7 @@
       <c r="I107" s="3"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="11"/>
+      <c r="A108" s="9"/>
       <c r="B108" s="6"/>
       <c r="C108" s="6"/>
       <c r="D108" s="3"/>
@@ -5704,7 +5705,7 @@
       <c r="I108" s="3"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" s="11"/>
+      <c r="A109" s="9"/>
       <c r="B109" s="6"/>
       <c r="C109" s="6"/>
       <c r="D109" s="3"/>
@@ -5715,7 +5716,7 @@
       <c r="I109" s="3"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A110" s="11"/>
+      <c r="A110" s="9"/>
       <c r="B110" s="6"/>
       <c r="C110" s="6"/>
       <c r="D110" s="3"/>
@@ -5726,7 +5727,7 @@
       <c r="I110" s="3"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A111" s="11"/>
+      <c r="A111" s="9"/>
       <c r="B111" s="6"/>
       <c r="C111" s="6"/>
       <c r="D111" s="3"/>
@@ -5737,7 +5738,7 @@
       <c r="I111" s="3"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A112" s="11"/>
+      <c r="A112" s="9"/>
       <c r="B112" s="6"/>
       <c r="C112" s="6"/>
       <c r="D112" s="3"/>
@@ -5748,7 +5749,7 @@
       <c r="I112" s="3"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A113" s="11"/>
+      <c r="A113" s="9"/>
       <c r="B113" s="6"/>
       <c r="C113" s="6"/>
       <c r="D113" s="3"/>
@@ -5759,7 +5760,7 @@
       <c r="I113" s="3"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A114" s="11"/>
+      <c r="A114" s="9"/>
       <c r="B114" s="6"/>
       <c r="C114" s="6"/>
       <c r="D114" s="3"/>
@@ -5770,7 +5771,7 @@
       <c r="I114" s="3"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A115" s="11"/>
+      <c r="A115" s="9"/>
       <c r="B115" s="6"/>
       <c r="C115" s="6"/>
       <c r="D115" s="3"/>
@@ -5781,7 +5782,7 @@
       <c r="I115" s="3"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A116" s="11"/>
+      <c r="A116" s="9"/>
       <c r="B116" s="6"/>
       <c r="C116" s="6"/>
       <c r="D116" s="3"/>
@@ -5792,7 +5793,7 @@
       <c r="I116" s="3"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A117" s="11"/>
+      <c r="A117" s="9"/>
       <c r="B117" s="6"/>
       <c r="C117" s="6"/>
       <c r="D117" s="3"/>
@@ -5803,7 +5804,7 @@
       <c r="I117" s="3"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A118" s="11"/>
+      <c r="A118" s="9"/>
       <c r="B118" s="6"/>
       <c r="C118" s="6"/>
       <c r="D118" s="3"/>
@@ -5814,7 +5815,7 @@
       <c r="I118" s="3"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A119" s="11"/>
+      <c r="A119" s="9"/>
       <c r="B119" s="6"/>
       <c r="C119" s="6"/>
       <c r="D119" s="3"/>
@@ -5825,7 +5826,7 @@
       <c r="I119" s="3"/>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A120" s="11"/>
+      <c r="A120" s="9"/>
       <c r="B120" s="6"/>
       <c r="C120" s="6"/>
       <c r="D120" s="3"/>
@@ -5836,7 +5837,7 @@
       <c r="I120" s="3"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A121" s="11"/>
+      <c r="A121" s="9"/>
       <c r="B121" s="6"/>
       <c r="C121" s="6"/>
       <c r="D121" s="3"/>
@@ -5847,7 +5848,7 @@
       <c r="I121" s="3"/>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A122" s="11"/>
+      <c r="A122" s="9"/>
       <c r="B122" s="6"/>
       <c r="C122" s="6"/>
       <c r="D122" s="3"/>
@@ -5858,7 +5859,7 @@
       <c r="I122" s="3"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A123" s="11"/>
+      <c r="A123" s="9"/>
       <c r="B123" s="6"/>
       <c r="C123" s="6"/>
       <c r="D123" s="3"/>
@@ -5869,7 +5870,7 @@
       <c r="I123" s="3"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A124" s="11"/>
+      <c r="A124" s="9"/>
       <c r="B124" s="6"/>
       <c r="C124" s="6"/>
       <c r="D124" s="3"/>
@@ -5880,7 +5881,7 @@
       <c r="I124" s="3"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A125" s="11"/>
+      <c r="A125" s="9"/>
       <c r="B125" s="6"/>
       <c r="C125" s="6"/>
       <c r="D125" s="3"/>
@@ -5891,7 +5892,7 @@
       <c r="I125" s="3"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A126" s="11"/>
+      <c r="A126" s="9"/>
       <c r="B126" s="6"/>
       <c r="C126" s="6"/>
       <c r="D126" s="3"/>
@@ -5902,7 +5903,7 @@
       <c r="I126" s="3"/>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A127" s="11"/>
+      <c r="A127" s="9"/>
       <c r="B127" s="6"/>
       <c r="C127" s="6"/>
       <c r="D127" s="3"/>
@@ -5913,7 +5914,7 @@
       <c r="I127" s="3"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A128" s="11"/>
+      <c r="A128" s="9"/>
       <c r="B128" s="6"/>
       <c r="C128" s="6"/>
       <c r="D128" s="3"/>
@@ -5924,7 +5925,7 @@
       <c r="I128" s="3"/>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A129" s="11"/>
+      <c r="A129" s="9"/>
       <c r="B129" s="6"/>
       <c r="C129" s="6"/>
       <c r="D129" s="3"/>
@@ -5935,7 +5936,7 @@
       <c r="I129" s="3"/>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A130" s="11"/>
+      <c r="A130" s="9"/>
       <c r="B130" s="6"/>
       <c r="C130" s="6"/>
       <c r="D130" s="3"/>
@@ -5946,7 +5947,7 @@
       <c r="I130" s="3"/>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A131" s="11"/>
+      <c r="A131" s="9"/>
       <c r="B131" s="6"/>
       <c r="C131" s="6"/>
       <c r="D131" s="3"/>
@@ -5957,7 +5958,7 @@
       <c r="I131" s="3"/>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A132" s="11"/>
+      <c r="A132" s="9"/>
       <c r="B132" s="6"/>
       <c r="C132" s="6"/>
       <c r="D132" s="3"/>
@@ -5968,7 +5969,7 @@
       <c r="I132" s="3"/>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A133" s="11"/>
+      <c r="A133" s="9"/>
       <c r="B133" s="6"/>
       <c r="C133" s="6"/>
       <c r="D133" s="3"/>
@@ -5979,7 +5980,7 @@
       <c r="I133" s="3"/>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A134" s="11"/>
+      <c r="A134" s="9"/>
       <c r="B134" s="6"/>
       <c r="C134" s="6"/>
       <c r="D134" s="3"/>
@@ -5990,7 +5991,7 @@
       <c r="I134" s="3"/>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A135" s="11"/>
+      <c r="A135" s="9"/>
       <c r="B135" s="6"/>
       <c r="C135" s="6"/>
       <c r="D135" s="3"/>
@@ -6001,7 +6002,7 @@
       <c r="I135" s="3"/>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A136" s="11"/>
+      <c r="A136" s="9"/>
       <c r="B136" s="6"/>
       <c r="C136" s="6"/>
       <c r="D136" s="3"/>
@@ -6012,7 +6013,7 @@
       <c r="I136" s="3"/>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A137" s="11"/>
+      <c r="A137" s="9"/>
       <c r="B137" s="6"/>
       <c r="C137" s="6"/>
       <c r="D137" s="3"/>
@@ -6023,7 +6024,7 @@
       <c r="I137" s="3"/>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A138" s="11"/>
+      <c r="A138" s="9"/>
       <c r="B138" s="6"/>
       <c r="C138" s="6"/>
       <c r="D138" s="3"/>
@@ -6034,7 +6035,7 @@
       <c r="I138" s="3"/>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A139" s="11"/>
+      <c r="A139" s="9"/>
       <c r="B139" s="6"/>
       <c r="C139" s="6"/>
       <c r="D139" s="3"/>
@@ -6045,7 +6046,7 @@
       <c r="I139" s="3"/>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A140" s="11"/>
+      <c r="A140" s="9"/>
       <c r="B140" s="6"/>
       <c r="C140" s="6"/>
       <c r="D140" s="3"/>
@@ -6056,7 +6057,7 @@
       <c r="I140" s="3"/>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A141" s="11"/>
+      <c r="A141" s="9"/>
       <c r="B141" s="6"/>
       <c r="C141" s="6"/>
       <c r="D141" s="3"/>
@@ -6067,7 +6068,7 @@
       <c r="I141" s="3"/>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A142" s="11"/>
+      <c r="A142" s="9"/>
       <c r="B142" s="6"/>
       <c r="C142" s="6"/>
       <c r="D142" s="3"/>
@@ -6078,7 +6079,7 @@
       <c r="I142" s="3"/>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A143" s="11"/>
+      <c r="A143" s="9"/>
       <c r="B143" s="6"/>
       <c r="C143" s="6"/>
       <c r="D143" s="3"/>
@@ -6089,7 +6090,7 @@
       <c r="I143" s="3"/>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A144" s="11"/>
+      <c r="A144" s="9"/>
       <c r="B144" s="6"/>
       <c r="C144" s="6"/>
       <c r="D144" s="3"/>
@@ -6100,7 +6101,7 @@
       <c r="I144" s="3"/>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A145" s="11"/>
+      <c r="A145" s="9"/>
       <c r="B145" s="6"/>
       <c r="C145" s="6"/>
       <c r="D145" s="3"/>
@@ -6111,7 +6112,7 @@
       <c r="I145" s="3"/>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A146" s="11"/>
+      <c r="A146" s="9"/>
       <c r="B146" s="6"/>
       <c r="C146" s="6"/>
       <c r="D146" s="3"/>
@@ -6122,7 +6123,7 @@
       <c r="I146" s="3"/>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A147" s="11"/>
+      <c r="A147" s="9"/>
       <c r="B147" s="6"/>
       <c r="C147" s="6"/>
       <c r="D147" s="3"/>
@@ -6133,7 +6134,7 @@
       <c r="I147" s="3"/>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A148" s="11"/>
+      <c r="A148" s="9"/>
       <c r="B148" s="6"/>
       <c r="C148" s="6"/>
       <c r="D148" s="3"/>
@@ -6144,7 +6145,7 @@
       <c r="I148" s="3"/>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A149" s="11"/>
+      <c r="A149" s="9"/>
       <c r="B149" s="6"/>
       <c r="C149" s="6"/>
       <c r="D149" s="3"/>
@@ -6155,7 +6156,7 @@
       <c r="I149" s="3"/>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A150" s="11"/>
+      <c r="A150" s="9"/>
       <c r="B150" s="6"/>
       <c r="C150" s="6"/>
       <c r="D150" s="3"/>
@@ -6166,7 +6167,7 @@
       <c r="I150" s="3"/>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A151" s="11"/>
+      <c r="A151" s="9"/>
       <c r="B151" s="6"/>
       <c r="C151" s="6"/>
       <c r="D151" s="3"/>
@@ -6177,7 +6178,7 @@
       <c r="I151" s="3"/>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A152" s="11"/>
+      <c r="A152" s="9"/>
       <c r="B152" s="6"/>
       <c r="C152" s="6"/>
       <c r="D152" s="3"/>
@@ -6188,7 +6189,7 @@
       <c r="I152" s="3"/>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A153" s="11"/>
+      <c r="A153" s="9"/>
       <c r="B153" s="6"/>
       <c r="C153" s="6"/>
       <c r="D153" s="3"/>
@@ -6199,7 +6200,7 @@
       <c r="I153" s="3"/>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A154" s="11"/>
+      <c r="A154" s="9"/>
       <c r="B154" s="6"/>
       <c r="C154" s="6"/>
       <c r="D154" s="3"/>
@@ -6210,7 +6211,7 @@
       <c r="I154" s="3"/>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A155" s="11"/>
+      <c r="A155" s="9"/>
       <c r="B155" s="6"/>
       <c r="C155" s="6"/>
       <c r="D155" s="3"/>
@@ -6221,7 +6222,7 @@
       <c r="I155" s="3"/>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A156" s="11"/>
+      <c r="A156" s="9"/>
       <c r="B156" s="6"/>
       <c r="C156" s="6"/>
       <c r="D156" s="3"/>
@@ -6232,7 +6233,7 @@
       <c r="I156" s="3"/>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A157" s="11"/>
+      <c r="A157" s="9"/>
       <c r="B157" s="6"/>
       <c r="C157" s="6"/>
       <c r="D157" s="3"/>
@@ -6243,7 +6244,7 @@
       <c r="I157" s="3"/>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A158" s="11"/>
+      <c r="A158" s="9"/>
       <c r="B158" s="6"/>
       <c r="C158" s="6"/>
       <c r="D158" s="3"/>
@@ -6254,7 +6255,7 @@
       <c r="I158" s="3"/>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A159" s="11"/>
+      <c r="A159" s="9"/>
       <c r="B159" s="6"/>
       <c r="C159" s="6"/>
       <c r="D159" s="3"/>
@@ -6265,7 +6266,7 @@
       <c r="I159" s="3"/>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A160" s="11"/>
+      <c r="A160" s="9"/>
       <c r="B160" s="6"/>
       <c r="C160" s="6"/>
       <c r="D160" s="3"/>
@@ -6276,7 +6277,7 @@
       <c r="I160" s="3"/>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A161" s="11"/>
+      <c r="A161" s="9"/>
       <c r="B161" s="6"/>
       <c r="C161" s="6"/>
       <c r="D161" s="3"/>
@@ -6287,7 +6288,7 @@
       <c r="I161" s="3"/>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A162" s="11"/>
+      <c r="A162" s="9"/>
       <c r="B162" s="6"/>
       <c r="C162" s="6"/>
       <c r="D162" s="3"/>
@@ -6298,7 +6299,7 @@
       <c r="I162" s="3"/>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A163" s="11"/>
+      <c r="A163" s="9"/>
       <c r="B163" s="6"/>
       <c r="C163" s="6"/>
       <c r="D163" s="3"/>
@@ -6309,7 +6310,7 @@
       <c r="I163" s="3"/>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A164" s="11"/>
+      <c r="A164" s="9"/>
       <c r="B164" s="6"/>
       <c r="C164" s="6"/>
       <c r="D164" s="3"/>
@@ -6320,7 +6321,7 @@
       <c r="I164" s="3"/>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A165" s="11"/>
+      <c r="A165" s="9"/>
       <c r="B165" s="6"/>
       <c r="C165" s="6"/>
       <c r="D165" s="3"/>
@@ -6331,7 +6332,7 @@
       <c r="I165" s="3"/>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A166" s="11"/>
+      <c r="A166" s="9"/>
       <c r="B166" s="6"/>
       <c r="C166" s="6"/>
       <c r="D166" s="3"/>
@@ -6342,7 +6343,7 @@
       <c r="I166" s="3"/>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A167" s="11"/>
+      <c r="A167" s="9"/>
       <c r="B167" s="6"/>
       <c r="C167" s="6"/>
       <c r="D167" s="3"/>
@@ -6353,7 +6354,7 @@
       <c r="I167" s="3"/>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A168" s="11"/>
+      <c r="A168" s="9"/>
       <c r="B168" s="6"/>
       <c r="C168" s="6"/>
       <c r="D168" s="3"/>
@@ -6364,7 +6365,7 @@
       <c r="I168" s="3"/>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A169" s="11"/>
+      <c r="A169" s="9"/>
       <c r="B169" s="6"/>
       <c r="C169" s="6"/>
       <c r="D169" s="3"/>
@@ -6375,7 +6376,7 @@
       <c r="I169" s="3"/>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A170" s="11"/>
+      <c r="A170" s="9"/>
       <c r="B170" s="6"/>
       <c r="C170" s="6"/>
       <c r="D170" s="3"/>
@@ -6386,7 +6387,7 @@
       <c r="I170" s="3"/>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A171" s="11"/>
+      <c r="A171" s="9"/>
       <c r="B171" s="6"/>
       <c r="C171" s="6"/>
       <c r="D171" s="3"/>
@@ -6397,7 +6398,7 @@
       <c r="I171" s="3"/>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A172" s="11"/>
+      <c r="A172" s="9"/>
       <c r="B172" s="6"/>
       <c r="C172" s="6"/>
       <c r="D172" s="3"/>
@@ -6408,7 +6409,7 @@
       <c r="I172" s="3"/>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A173" s="11"/>
+      <c r="A173" s="9"/>
       <c r="B173" s="6"/>
       <c r="C173" s="6"/>
       <c r="D173" s="3"/>
@@ -6419,7 +6420,7 @@
       <c r="I173" s="3"/>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A174" s="11"/>
+      <c r="A174" s="9"/>
       <c r="B174" s="6"/>
       <c r="C174" s="6"/>
       <c r="D174" s="3"/>
@@ -6430,7 +6431,7 @@
       <c r="I174" s="3"/>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A175" s="11"/>
+      <c r="A175" s="9"/>
       <c r="B175" s="6"/>
       <c r="C175" s="6"/>
       <c r="D175" s="3"/>
@@ -6441,7 +6442,7 @@
       <c r="I175" s="3"/>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A176" s="11"/>
+      <c r="A176" s="9"/>
       <c r="B176" s="6"/>
       <c r="C176" s="6"/>
       <c r="D176" s="3"/>
@@ -6452,7 +6453,7 @@
       <c r="I176" s="3"/>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A177" s="11"/>
+      <c r="A177" s="9"/>
       <c r="B177" s="6"/>
       <c r="C177" s="6"/>
       <c r="D177" s="3"/>
@@ -6463,7 +6464,7 @@
       <c r="I177" s="3"/>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A178" s="11"/>
+      <c r="A178" s="9"/>
       <c r="B178" s="6"/>
       <c r="C178" s="6"/>
       <c r="D178" s="3"/>
@@ -6474,7 +6475,7 @@
       <c r="I178" s="3"/>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A179" s="11"/>
+      <c r="A179" s="9"/>
       <c r="B179" s="6"/>
       <c r="C179" s="6"/>
       <c r="D179" s="3"/>
@@ -6485,7 +6486,7 @@
       <c r="I179" s="3"/>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A180" s="11"/>
+      <c r="A180" s="9"/>
       <c r="B180" s="6"/>
       <c r="C180" s="6"/>
       <c r="D180" s="3"/>
@@ -6496,7 +6497,7 @@
       <c r="I180" s="3"/>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A181" s="11"/>
+      <c r="A181" s="9"/>
       <c r="B181" s="6"/>
       <c r="C181" s="6"/>
       <c r="D181" s="3"/>
@@ -6507,7 +6508,7 @@
       <c r="I181" s="3"/>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A182" s="11"/>
+      <c r="A182" s="9"/>
       <c r="B182" s="6"/>
       <c r="C182" s="6"/>
       <c r="D182" s="3"/>
@@ -6518,7 +6519,7 @@
       <c r="I182" s="3"/>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A183" s="11"/>
+      <c r="A183" s="9"/>
       <c r="B183" s="6"/>
       <c r="C183" s="6"/>
       <c r="D183" s="3"/>
@@ -6529,7 +6530,7 @@
       <c r="I183" s="3"/>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A184" s="11"/>
+      <c r="A184" s="9"/>
       <c r="B184" s="6"/>
       <c r="C184" s="6"/>
       <c r="D184" s="3"/>
@@ -6540,7 +6541,7 @@
       <c r="I184" s="3"/>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A185" s="11"/>
+      <c r="A185" s="9"/>
       <c r="B185" s="6"/>
       <c r="C185" s="6"/>
       <c r="D185" s="3"/>
@@ -6551,7 +6552,7 @@
       <c r="I185" s="3"/>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A186" s="11"/>
+      <c r="A186" s="9"/>
       <c r="B186" s="6"/>
       <c r="C186" s="6"/>
       <c r="D186" s="3"/>
@@ -6562,7 +6563,7 @@
       <c r="I186" s="3"/>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A187" s="11"/>
+      <c r="A187" s="9"/>
       <c r="B187" s="6"/>
       <c r="C187" s="6"/>
       <c r="D187" s="3"/>
@@ -6573,7 +6574,7 @@
       <c r="I187" s="3"/>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A188" s="11"/>
+      <c r="A188" s="9"/>
       <c r="B188" s="6"/>
       <c r="C188" s="6"/>
       <c r="D188" s="3"/>
@@ -6584,7 +6585,7 @@
       <c r="I188" s="3"/>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A189" s="11"/>
+      <c r="A189" s="9"/>
       <c r="B189" s="6"/>
       <c r="C189" s="6"/>
       <c r="D189" s="3"/>
@@ -6595,7 +6596,7 @@
       <c r="I189" s="3"/>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A190" s="11"/>
+      <c r="A190" s="9"/>
       <c r="B190" s="6"/>
       <c r="C190" s="6"/>
       <c r="D190" s="3"/>
@@ -6606,7 +6607,7 @@
       <c r="I190" s="3"/>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A191" s="11"/>
+      <c r="A191" s="9"/>
       <c r="B191" s="6"/>
       <c r="C191" s="6"/>
       <c r="D191" s="3"/>
@@ -6617,7 +6618,7 @@
       <c r="I191" s="3"/>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A192" s="11"/>
+      <c r="A192" s="9"/>
       <c r="B192" s="6"/>
       <c r="C192" s="6"/>
       <c r="D192" s="3"/>
@@ -6628,7 +6629,7 @@
       <c r="I192" s="3"/>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A193" s="11"/>
+      <c r="A193" s="9"/>
       <c r="B193" s="6"/>
       <c r="C193" s="6"/>
       <c r="D193" s="3"/>
@@ -6639,7 +6640,7 @@
       <c r="I193" s="3"/>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A194" s="11"/>
+      <c r="A194" s="9"/>
       <c r="B194" s="6"/>
       <c r="C194" s="6"/>
       <c r="D194" s="3"/>
@@ -6650,7 +6651,7 @@
       <c r="I194" s="3"/>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A195" s="11"/>
+      <c r="A195" s="9"/>
       <c r="B195" s="6"/>
       <c r="C195" s="6"/>
       <c r="D195" s="3"/>
@@ -6661,7 +6662,7 @@
       <c r="I195" s="3"/>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A196" s="11"/>
+      <c r="A196" s="9"/>
       <c r="B196" s="6"/>
       <c r="C196" s="6"/>
       <c r="D196" s="3"/>
@@ -6672,7 +6673,7 @@
       <c r="I196" s="3"/>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A197" s="11"/>
+      <c r="A197" s="9"/>
       <c r="B197" s="6"/>
       <c r="C197" s="6"/>
       <c r="D197" s="3"/>
@@ -6683,7 +6684,7 @@
       <c r="I197" s="3"/>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A198" s="11"/>
+      <c r="A198" s="9"/>
       <c r="B198" s="6"/>
       <c r="C198" s="6"/>
       <c r="D198" s="3"/>
@@ -6694,7 +6695,7 @@
       <c r="I198" s="3"/>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A199" s="11"/>
+      <c r="A199" s="9"/>
       <c r="B199" s="6"/>
       <c r="C199" s="6"/>
       <c r="D199" s="3"/>
@@ -6705,7 +6706,7 @@
       <c r="I199" s="3"/>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A200" s="11"/>
+      <c r="A200" s="9"/>
       <c r="B200" s="6"/>
       <c r="C200" s="6"/>
       <c r="D200" s="3"/>
@@ -6716,7 +6717,7 @@
       <c r="I200" s="3"/>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A201" s="11"/>
+      <c r="A201" s="9"/>
       <c r="B201" s="6"/>
       <c r="C201" s="6"/>
       <c r="D201" s="3"/>
@@ -6727,7 +6728,7 @@
       <c r="I201" s="3"/>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A202" s="11"/>
+      <c r="A202" s="9"/>
       <c r="B202" s="6"/>
       <c r="C202" s="6"/>
       <c r="D202" s="3"/>
@@ -6738,7 +6739,7 @@
       <c r="I202" s="3"/>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A203" s="11"/>
+      <c r="A203" s="9"/>
       <c r="B203" s="6"/>
       <c r="C203" s="6"/>
       <c r="D203" s="3"/>
@@ -6749,7 +6750,7 @@
       <c r="I203" s="3"/>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A204" s="11"/>
+      <c r="A204" s="9"/>
       <c r="B204" s="6"/>
       <c r="C204" s="6"/>
       <c r="D204" s="3"/>
@@ -6760,7 +6761,7 @@
       <c r="I204" s="3"/>
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A205" s="11"/>
+      <c r="A205" s="9"/>
       <c r="B205" s="6"/>
       <c r="C205" s="6"/>
       <c r="D205" s="3"/>
@@ -6771,7 +6772,7 @@
       <c r="I205" s="3"/>
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A206" s="11"/>
+      <c r="A206" s="9"/>
       <c r="B206" s="6"/>
       <c r="C206" s="6"/>
       <c r="D206" s="3"/>
@@ -6782,7 +6783,7 @@
       <c r="I206" s="3"/>
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A207" s="11"/>
+      <c r="A207" s="9"/>
       <c r="B207" s="6"/>
       <c r="C207" s="6"/>
       <c r="D207" s="3"/>
@@ -6793,7 +6794,7 @@
       <c r="I207" s="3"/>
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A208" s="11"/>
+      <c r="A208" s="9"/>
       <c r="B208" s="6"/>
       <c r="C208" s="6"/>
       <c r="D208" s="3"/>
@@ -6804,7 +6805,7 @@
       <c r="I208" s="3"/>
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A209" s="11"/>
+      <c r="A209" s="9"/>
       <c r="B209" s="6"/>
       <c r="C209" s="6"/>
       <c r="D209" s="3"/>
@@ -6815,7 +6816,7 @@
       <c r="I209" s="3"/>
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A210" s="11"/>
+      <c r="A210" s="9"/>
       <c r="B210" s="6"/>
       <c r="C210" s="6"/>
       <c r="D210" s="3"/>
@@ -6826,7 +6827,7 @@
       <c r="I210" s="3"/>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A211" s="11"/>
+      <c r="A211" s="9"/>
       <c r="B211" s="6"/>
       <c r="C211" s="6"/>
       <c r="D211" s="3"/>
@@ -6837,7 +6838,7 @@
       <c r="I211" s="3"/>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A212" s="11"/>
+      <c r="A212" s="9"/>
       <c r="B212" s="6"/>
       <c r="C212" s="6"/>
       <c r="D212" s="3"/>
@@ -6848,7 +6849,7 @@
       <c r="I212" s="3"/>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A213" s="11"/>
+      <c r="A213" s="9"/>
       <c r="B213" s="6"/>
       <c r="C213" s="6"/>
       <c r="D213" s="3"/>
@@ -6859,7 +6860,7 @@
       <c r="I213" s="3"/>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A214" s="11"/>
+      <c r="A214" s="9"/>
       <c r="B214" s="6"/>
       <c r="C214" s="6"/>
       <c r="D214" s="3"/>
@@ -6870,7 +6871,7 @@
       <c r="I214" s="3"/>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A215" s="11"/>
+      <c r="A215" s="9"/>
       <c r="B215" s="6"/>
       <c r="C215" s="6"/>
       <c r="D215" s="3"/>
@@ -6881,7 +6882,7 @@
       <c r="I215" s="3"/>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A216" s="11"/>
+      <c r="A216" s="9"/>
       <c r="B216" s="6"/>
       <c r="C216" s="6"/>
       <c r="D216" s="3"/>
@@ -6892,7 +6893,7 @@
       <c r="I216" s="3"/>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A217" s="11"/>
+      <c r="A217" s="9"/>
       <c r="B217" s="6"/>
       <c r="C217" s="6"/>
       <c r="D217" s="3"/>
@@ -6903,7 +6904,7 @@
       <c r="I217" s="3"/>
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A218" s="11"/>
+      <c r="A218" s="9"/>
       <c r="B218" s="6"/>
       <c r="C218" s="6"/>
       <c r="D218" s="3"/>
@@ -6914,7 +6915,7 @@
       <c r="I218" s="3"/>
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A219" s="11"/>
+      <c r="A219" s="9"/>
       <c r="B219" s="6"/>
       <c r="C219" s="6"/>
       <c r="D219" s="3"/>
@@ -6925,7 +6926,7 @@
       <c r="I219" s="3"/>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A220" s="11"/>
+      <c r="A220" s="9"/>
       <c r="B220" s="6"/>
       <c r="C220" s="6"/>
       <c r="D220" s="3"/>
@@ -6936,7 +6937,7 @@
       <c r="I220" s="3"/>
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A221" s="11"/>
+      <c r="A221" s="9"/>
       <c r="B221" s="6"/>
       <c r="C221" s="6"/>
       <c r="D221" s="3"/>
@@ -6947,7 +6948,7 @@
       <c r="I221" s="3"/>
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A222" s="11"/>
+      <c r="A222" s="9"/>
       <c r="B222" s="6"/>
       <c r="C222" s="6"/>
       <c r="D222" s="3"/>
@@ -6958,7 +6959,7 @@
       <c r="I222" s="3"/>
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A223" s="11"/>
+      <c r="A223" s="9"/>
       <c r="B223" s="6"/>
       <c r="C223" s="6"/>
       <c r="D223" s="3"/>
@@ -6969,7 +6970,7 @@
       <c r="I223" s="3"/>
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A224" s="11"/>
+      <c r="A224" s="9"/>
       <c r="B224" s="6"/>
       <c r="C224" s="6"/>
       <c r="D224" s="3"/>
@@ -6980,7 +6981,7 @@
       <c r="I224" s="3"/>
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A225" s="11"/>
+      <c r="A225" s="9"/>
       <c r="B225" s="6"/>
       <c r="C225" s="6"/>
       <c r="D225" s="3"/>
@@ -6991,7 +6992,7 @@
       <c r="I225" s="3"/>
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A226" s="11"/>
+      <c r="A226" s="9"/>
       <c r="B226" s="6"/>
       <c r="C226" s="6"/>
       <c r="D226" s="3"/>
@@ -7002,7 +7003,7 @@
       <c r="I226" s="3"/>
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A227" s="11"/>
+      <c r="A227" s="9"/>
       <c r="B227" s="6"/>
       <c r="C227" s="6"/>
       <c r="D227" s="3"/>
@@ -7013,7 +7014,7 @@
       <c r="I227" s="3"/>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A228" s="11"/>
+      <c r="A228" s="9"/>
       <c r="B228" s="6"/>
       <c r="C228" s="6"/>
       <c r="D228" s="3"/>
@@ -7024,7 +7025,7 @@
       <c r="I228" s="3"/>
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A229" s="11"/>
+      <c r="A229" s="9"/>
       <c r="B229" s="6"/>
       <c r="C229" s="6"/>
       <c r="D229" s="3"/>
@@ -7035,7 +7036,7 @@
       <c r="I229" s="3"/>
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A230" s="11"/>
+      <c r="A230" s="9"/>
       <c r="B230" s="6"/>
       <c r="C230" s="6"/>
       <c r="D230" s="3"/>
@@ -7046,7 +7047,7 @@
       <c r="I230" s="3"/>
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A231" s="11"/>
+      <c r="A231" s="9"/>
       <c r="B231" s="6"/>
       <c r="C231" s="6"/>
       <c r="D231" s="3"/>
@@ -7057,7 +7058,7 @@
       <c r="I231" s="3"/>
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A232" s="11"/>
+      <c r="A232" s="9"/>
       <c r="B232" s="6"/>
       <c r="C232" s="6"/>
       <c r="D232" s="3"/>
@@ -7068,7 +7069,7 @@
       <c r="I232" s="3"/>
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A233" s="11"/>
+      <c r="A233" s="9"/>
       <c r="B233" s="6"/>
       <c r="C233" s="6"/>
       <c r="D233" s="3"/>
@@ -7079,7 +7080,7 @@
       <c r="I233" s="3"/>
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A234" s="11"/>
+      <c r="A234" s="9"/>
       <c r="B234" s="6"/>
       <c r="C234" s="6"/>
       <c r="D234" s="3"/>
@@ -7090,7 +7091,7 @@
       <c r="I234" s="3"/>
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A235" s="11"/>
+      <c r="A235" s="9"/>
       <c r="B235" s="6"/>
       <c r="C235" s="6"/>
       <c r="D235" s="3"/>
@@ -7101,7 +7102,7 @@
       <c r="I235" s="3"/>
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A236" s="11"/>
+      <c r="A236" s="9"/>
       <c r="B236" s="6"/>
       <c r="C236" s="6"/>
       <c r="D236" s="3"/>
@@ -7112,7 +7113,7 @@
       <c r="I236" s="3"/>
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A237" s="11"/>
+      <c r="A237" s="9"/>
       <c r="B237" s="6"/>
       <c r="C237" s="6"/>
       <c r="D237" s="3"/>
@@ -7123,7 +7124,7 @@
       <c r="I237" s="3"/>
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A238" s="11"/>
+      <c r="A238" s="9"/>
       <c r="B238" s="6"/>
       <c r="C238" s="6"/>
       <c r="D238" s="3"/>
@@ -7134,7 +7135,7 @@
       <c r="I238" s="3"/>
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A239" s="11"/>
+      <c r="A239" s="9"/>
       <c r="B239" s="6"/>
       <c r="C239" s="6"/>
       <c r="D239" s="3"/>
@@ -7145,7 +7146,7 @@
       <c r="I239" s="3"/>
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A240" s="11"/>
+      <c r="A240" s="9"/>
       <c r="B240" s="6"/>
       <c r="C240" s="6"/>
       <c r="D240" s="3"/>
@@ -7156,7 +7157,7 @@
       <c r="I240" s="3"/>
     </row>
     <row r="241" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A241" s="11"/>
+      <c r="A241" s="9"/>
       <c r="B241" s="6"/>
       <c r="C241" s="6"/>
       <c r="D241" s="3"/>
@@ -7167,7 +7168,7 @@
       <c r="I241" s="3"/>
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A242" s="11"/>
+      <c r="A242" s="9"/>
       <c r="B242" s="6"/>
       <c r="C242" s="6"/>
       <c r="D242" s="3"/>
@@ -7178,7 +7179,7 @@
       <c r="I242" s="3"/>
     </row>
     <row r="243" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A243" s="11"/>
+      <c r="A243" s="9"/>
       <c r="B243" s="6"/>
       <c r="C243" s="6"/>
       <c r="D243" s="3"/>
@@ -7189,7 +7190,7 @@
       <c r="I243" s="3"/>
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A244" s="11"/>
+      <c r="A244" s="9"/>
       <c r="B244" s="6"/>
       <c r="C244" s="6"/>
       <c r="D244" s="3"/>
@@ -7200,7 +7201,7 @@
       <c r="I244" s="3"/>
     </row>
     <row r="245" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A245" s="11"/>
+      <c r="A245" s="9"/>
       <c r="B245" s="6"/>
       <c r="C245" s="6"/>
       <c r="D245" s="3"/>
@@ -7211,7 +7212,7 @@
       <c r="I245" s="3"/>
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A246" s="11"/>
+      <c r="A246" s="9"/>
       <c r="B246" s="6"/>
       <c r="C246" s="6"/>
       <c r="D246" s="3"/>
@@ -7222,7 +7223,7 @@
       <c r="I246" s="3"/>
     </row>
     <row r="247" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A247" s="11"/>
+      <c r="A247" s="9"/>
       <c r="B247" s="6"/>
       <c r="C247" s="6"/>
       <c r="D247" s="3"/>
@@ -7233,7 +7234,7 @@
       <c r="I247" s="3"/>
     </row>
     <row r="248" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A248" s="11"/>
+      <c r="A248" s="9"/>
       <c r="B248" s="6"/>
       <c r="C248" s="6"/>
       <c r="D248" s="3"/>
@@ -7244,7 +7245,7 @@
       <c r="I248" s="3"/>
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A249" s="11"/>
+      <c r="A249" s="9"/>
       <c r="B249" s="6"/>
       <c r="C249" s="6"/>
       <c r="D249" s="3"/>
@@ -7255,7 +7256,7 @@
       <c r="I249" s="3"/>
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A250" s="11"/>
+      <c r="A250" s="9"/>
       <c r="B250" s="6"/>
       <c r="C250" s="6"/>
       <c r="D250" s="3"/>
@@ -7266,7 +7267,7 @@
       <c r="I250" s="3"/>
     </row>
     <row r="251" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A251" s="11"/>
+      <c r="A251" s="9"/>
       <c r="B251" s="6"/>
       <c r="C251" s="6"/>
       <c r="D251" s="3"/>
@@ -7277,7 +7278,7 @@
       <c r="I251" s="3"/>
     </row>
     <row r="252" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A252" s="11"/>
+      <c r="A252" s="9"/>
       <c r="B252" s="6"/>
       <c r="C252" s="6"/>
       <c r="D252" s="3"/>
@@ -7288,7 +7289,7 @@
       <c r="I252" s="3"/>
     </row>
     <row r="253" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A253" s="11"/>
+      <c r="A253" s="9"/>
       <c r="B253" s="6"/>
       <c r="C253" s="6"/>
       <c r="D253" s="3"/>
@@ -7299,7 +7300,7 @@
       <c r="I253" s="3"/>
     </row>
     <row r="254" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A254" s="11"/>
+      <c r="A254" s="9"/>
       <c r="B254" s="6"/>
       <c r="C254" s="6"/>
       <c r="D254" s="3"/>
@@ -7310,7 +7311,7 @@
       <c r="I254" s="3"/>
     </row>
     <row r="255" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A255" s="11"/>
+      <c r="A255" s="9"/>
       <c r="B255" s="6"/>
       <c r="C255" s="6"/>
       <c r="D255" s="3"/>
@@ -7321,7 +7322,7 @@
       <c r="I255" s="3"/>
     </row>
     <row r="256" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A256" s="11"/>
+      <c r="A256" s="9"/>
       <c r="B256" s="6"/>
       <c r="C256" s="6"/>
       <c r="D256" s="3"/>
@@ -7332,7 +7333,7 @@
       <c r="I256" s="3"/>
     </row>
     <row r="257" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A257" s="11"/>
+      <c r="A257" s="9"/>
       <c r="B257" s="6"/>
       <c r="C257" s="6"/>
       <c r="D257" s="3"/>
@@ -7343,7 +7344,7 @@
       <c r="I257" s="3"/>
     </row>
     <row r="258" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A258" s="11"/>
+      <c r="A258" s="9"/>
       <c r="B258" s="6"/>
       <c r="C258" s="6"/>
       <c r="D258" s="3"/>
@@ -7354,7 +7355,7 @@
       <c r="I258" s="3"/>
     </row>
     <row r="259" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A259" s="11"/>
+      <c r="A259" s="9"/>
       <c r="B259" s="6"/>
       <c r="C259" s="6"/>
       <c r="D259" s="3"/>
@@ -7365,7 +7366,7 @@
       <c r="I259" s="3"/>
     </row>
     <row r="260" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A260" s="11"/>
+      <c r="A260" s="9"/>
       <c r="B260" s="6"/>
       <c r="C260" s="6"/>
       <c r="D260" s="3"/>
@@ -7376,7 +7377,7 @@
       <c r="I260" s="3"/>
     </row>
     <row r="261" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A261" s="11"/>
+      <c r="A261" s="9"/>
       <c r="B261" s="6"/>
       <c r="C261" s="6"/>
       <c r="D261" s="3"/>
@@ -7387,7 +7388,7 @@
       <c r="I261" s="3"/>
     </row>
     <row r="262" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A262" s="11"/>
+      <c r="A262" s="9"/>
       <c r="B262" s="6"/>
       <c r="C262" s="6"/>
       <c r="D262" s="3"/>
@@ -7398,7 +7399,7 @@
       <c r="I262" s="3"/>
     </row>
     <row r="263" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A263" s="11"/>
+      <c r="A263" s="9"/>
       <c r="B263" s="6"/>
       <c r="C263" s="6"/>
       <c r="D263" s="3"/>
@@ -7409,7 +7410,7 @@
       <c r="I263" s="3"/>
     </row>
     <row r="264" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A264" s="11"/>
+      <c r="A264" s="9"/>
       <c r="B264" s="6"/>
       <c r="C264" s="6"/>
       <c r="D264" s="3"/>
@@ -7420,7 +7421,7 @@
       <c r="I264" s="3"/>
     </row>
     <row r="265" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A265" s="11"/>
+      <c r="A265" s="9"/>
       <c r="B265" s="6"/>
       <c r="C265" s="6"/>
       <c r="D265" s="3"/>
@@ -7431,7 +7432,7 @@
       <c r="I265" s="3"/>
     </row>
     <row r="266" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A266" s="11"/>
+      <c r="A266" s="9"/>
       <c r="B266" s="6"/>
       <c r="C266" s="6"/>
       <c r="D266" s="3"/>
@@ -7442,7 +7443,7 @@
       <c r="I266" s="3"/>
     </row>
     <row r="267" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A267" s="11"/>
+      <c r="A267" s="9"/>
       <c r="B267" s="6"/>
       <c r="C267" s="6"/>
       <c r="D267" s="3"/>
@@ -7453,7 +7454,7 @@
       <c r="I267" s="3"/>
     </row>
     <row r="268" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A268" s="11"/>
+      <c r="A268" s="9"/>
       <c r="B268" s="6"/>
       <c r="C268" s="6"/>
       <c r="D268" s="3"/>
@@ -7464,7 +7465,7 @@
       <c r="I268" s="3"/>
     </row>
     <row r="269" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A269" s="11"/>
+      <c r="A269" s="9"/>
       <c r="B269" s="6"/>
       <c r="C269" s="6"/>
       <c r="D269" s="3"/>
@@ -7475,7 +7476,7 @@
       <c r="I269" s="3"/>
     </row>
     <row r="270" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A270" s="11"/>
+      <c r="A270" s="9"/>
       <c r="B270" s="6"/>
       <c r="C270" s="6"/>
       <c r="D270" s="3"/>
@@ -7486,7 +7487,7 @@
       <c r="I270" s="3"/>
     </row>
     <row r="271" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A271" s="11"/>
+      <c r="A271" s="9"/>
       <c r="B271" s="6"/>
       <c r="C271" s="6"/>
       <c r="D271" s="3"/>
@@ -7497,7 +7498,7 @@
       <c r="I271" s="3"/>
     </row>
     <row r="272" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A272" s="11"/>
+      <c r="A272" s="9"/>
       <c r="B272" s="6"/>
       <c r="C272" s="6"/>
       <c r="D272" s="3"/>
@@ -7508,7 +7509,7 @@
       <c r="I272" s="3"/>
     </row>
     <row r="273" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A273" s="11"/>
+      <c r="A273" s="9"/>
       <c r="B273" s="6"/>
       <c r="C273" s="6"/>
       <c r="D273" s="3"/>
@@ -7519,7 +7520,7 @@
       <c r="I273" s="3"/>
     </row>
     <row r="274" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A274" s="11"/>
+      <c r="A274" s="9"/>
       <c r="B274" s="6"/>
       <c r="C274" s="6"/>
       <c r="D274" s="3"/>
@@ -7530,7 +7531,7 @@
       <c r="I274" s="3"/>
     </row>
     <row r="275" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A275" s="11"/>
+      <c r="A275" s="9"/>
       <c r="B275" s="6"/>
       <c r="C275" s="6"/>
       <c r="D275" s="3"/>
@@ -7541,7 +7542,7 @@
       <c r="I275" s="3"/>
     </row>
     <row r="276" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A276" s="11"/>
+      <c r="A276" s="9"/>
       <c r="B276" s="6"/>
       <c r="C276" s="6"/>
       <c r="D276" s="3"/>
@@ -7552,7 +7553,7 @@
       <c r="I276" s="3"/>
     </row>
     <row r="277" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A277" s="11"/>
+      <c r="A277" s="9"/>
       <c r="B277" s="6"/>
       <c r="C277" s="6"/>
       <c r="D277" s="3"/>
@@ -7563,7 +7564,7 @@
       <c r="I277" s="3"/>
     </row>
     <row r="278" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A278" s="11"/>
+      <c r="A278" s="9"/>
       <c r="B278" s="6"/>
       <c r="C278" s="6"/>
       <c r="D278" s="3"/>
@@ -7574,7 +7575,7 @@
       <c r="I278" s="3"/>
     </row>
     <row r="279" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A279" s="11"/>
+      <c r="A279" s="9"/>
       <c r="B279" s="6"/>
       <c r="C279" s="6"/>
       <c r="D279" s="3"/>
@@ -7585,7 +7586,7 @@
       <c r="I279" s="3"/>
     </row>
     <row r="280" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A280" s="11"/>
+      <c r="A280" s="9"/>
       <c r="B280" s="6"/>
       <c r="C280" s="6"/>
       <c r="D280" s="3"/>
@@ -7596,7 +7597,7 @@
       <c r="I280" s="3"/>
     </row>
     <row r="281" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A281" s="11"/>
+      <c r="A281" s="9"/>
       <c r="B281" s="6"/>
       <c r="C281" s="6"/>
       <c r="D281" s="3"/>
@@ -7607,7 +7608,7 @@
       <c r="I281" s="3"/>
     </row>
     <row r="282" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A282" s="11"/>
+      <c r="A282" s="9"/>
       <c r="B282" s="6"/>
       <c r="C282" s="6"/>
       <c r="D282" s="3"/>
@@ -7618,7 +7619,7 @@
       <c r="I282" s="3"/>
     </row>
     <row r="283" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A283" s="11"/>
+      <c r="A283" s="9"/>
       <c r="B283" s="6"/>
       <c r="C283" s="6"/>
       <c r="D283" s="3"/>
@@ -7629,7 +7630,7 @@
       <c r="I283" s="3"/>
     </row>
     <row r="284" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A284" s="11"/>
+      <c r="A284" s="9"/>
       <c r="B284" s="3"/>
       <c r="C284" s="3"/>
       <c r="D284" s="3"/>
@@ -7640,7 +7641,7 @@
       <c r="I284" s="3"/>
     </row>
     <row r="285" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A285" s="11"/>
+      <c r="A285" s="9"/>
       <c r="B285" s="3"/>
       <c r="C285" s="3"/>
       <c r="D285" s="3"/>
@@ -7651,7 +7652,7 @@
       <c r="I285" s="3"/>
     </row>
     <row r="286" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A286" s="11"/>
+      <c r="A286" s="9"/>
       <c r="B286" s="3"/>
       <c r="C286" s="3"/>
       <c r="D286" s="3"/>
@@ -7662,7 +7663,7 @@
       <c r="I286" s="3"/>
     </row>
     <row r="287" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A287" s="11"/>
+      <c r="A287" s="9"/>
       <c r="B287" s="3"/>
       <c r="C287" s="3"/>
       <c r="D287" s="3"/>
@@ -7673,7 +7674,7 @@
       <c r="I287" s="3"/>
     </row>
     <row r="288" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A288" s="11"/>
+      <c r="A288" s="9"/>
       <c r="B288" s="3"/>
       <c r="C288" s="3"/>
       <c r="D288" s="3"/>
@@ -7684,7 +7685,7 @@
       <c r="I288" s="3"/>
     </row>
     <row r="289" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A289" s="11"/>
+      <c r="A289" s="9"/>
       <c r="B289" s="3"/>
       <c r="C289" s="3"/>
       <c r="D289" s="3"/>
@@ -7695,7 +7696,7 @@
       <c r="I289" s="3"/>
     </row>
     <row r="290" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A290" s="11"/>
+      <c r="A290" s="9"/>
       <c r="B290" s="3"/>
       <c r="C290" s="3"/>
       <c r="D290" s="3"/>
@@ -7706,7 +7707,7 @@
       <c r="I290" s="3"/>
     </row>
     <row r="291" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A291" s="11"/>
+      <c r="A291" s="9"/>
       <c r="B291" s="3"/>
       <c r="C291" s="3"/>
       <c r="D291" s="3"/>
@@ -7717,7 +7718,7 @@
       <c r="I291" s="3"/>
     </row>
     <row r="292" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A292" s="11"/>
+      <c r="A292" s="9"/>
       <c r="B292" s="3"/>
       <c r="C292" s="3"/>
       <c r="D292" s="3"/>
@@ -7728,7 +7729,7 @@
       <c r="I292" s="3"/>
     </row>
     <row r="293" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A293" s="11"/>
+      <c r="A293" s="9"/>
       <c r="B293" s="3"/>
       <c r="C293" s="3"/>
       <c r="D293" s="3"/>
@@ -7739,7 +7740,7 @@
       <c r="I293" s="3"/>
     </row>
     <row r="294" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A294" s="11"/>
+      <c r="A294" s="9"/>
       <c r="B294" s="3"/>
       <c r="C294" s="3"/>
       <c r="D294" s="3"/>
@@ -7750,7 +7751,7 @@
       <c r="I294" s="3"/>
     </row>
     <row r="295" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A295" s="11"/>
+      <c r="A295" s="9"/>
       <c r="B295" s="3"/>
       <c r="C295" s="3"/>
       <c r="D295" s="3"/>
@@ -7761,7 +7762,7 @@
       <c r="I295" s="3"/>
     </row>
     <row r="296" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A296" s="11"/>
+      <c r="A296" s="9"/>
       <c r="B296" s="3"/>
       <c r="C296" s="3"/>
       <c r="D296" s="3"/>
@@ -7772,7 +7773,7 @@
       <c r="I296" s="3"/>
     </row>
     <row r="297" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A297" s="11"/>
+      <c r="A297" s="9"/>
       <c r="B297" s="3"/>
       <c r="C297" s="3"/>
       <c r="D297" s="3"/>
@@ -7783,7 +7784,7 @@
       <c r="I297" s="3"/>
     </row>
     <row r="298" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A298" s="11"/>
+      <c r="A298" s="9"/>
       <c r="B298" s="3"/>
       <c r="C298" s="3"/>
       <c r="D298" s="3"/>
@@ -7794,7 +7795,7 @@
       <c r="I298" s="3"/>
     </row>
     <row r="299" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A299" s="11"/>
+      <c r="A299" s="9"/>
       <c r="B299" s="3"/>
       <c r="C299" s="3"/>
       <c r="D299" s="3"/>
@@ -7805,7 +7806,7 @@
       <c r="I299" s="3"/>
     </row>
     <row r="300" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A300" s="11"/>
+      <c r="A300" s="9"/>
       <c r="B300" s="3"/>
       <c r="C300" s="3"/>
       <c r="D300" s="3"/>
@@ -7816,7 +7817,7 @@
       <c r="I300" s="3"/>
     </row>
     <row r="301" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A301" s="11"/>
+      <c r="A301" s="9"/>
       <c r="B301" s="3"/>
       <c r="C301" s="3"/>
       <c r="D301" s="3"/>
@@ -7827,7 +7828,7 @@
       <c r="I301" s="3"/>
     </row>
     <row r="302" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A302" s="11"/>
+      <c r="A302" s="9"/>
       <c r="B302" s="3"/>
       <c r="C302" s="3"/>
       <c r="D302" s="3"/>
@@ -7838,7 +7839,7 @@
       <c r="I302" s="3"/>
     </row>
     <row r="303" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A303" s="11"/>
+      <c r="A303" s="9"/>
       <c r="B303" s="3"/>
       <c r="C303" s="3"/>
       <c r="D303" s="3"/>
@@ -7849,7 +7850,7 @@
       <c r="I303" s="3"/>
     </row>
     <row r="304" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A304" s="11"/>
+      <c r="A304" s="9"/>
       <c r="B304" s="3"/>
       <c r="C304" s="3"/>
       <c r="D304" s="3"/>
@@ -7860,7 +7861,7 @@
       <c r="I304" s="3"/>
     </row>
     <row r="305" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A305" s="11"/>
+      <c r="A305" s="9"/>
       <c r="B305" s="3"/>
       <c r="C305" s="3"/>
       <c r="D305" s="3"/>
@@ -7871,7 +7872,7 @@
       <c r="I305" s="3"/>
     </row>
     <row r="306" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A306" s="11"/>
+      <c r="A306" s="9"/>
       <c r="B306" s="3"/>
       <c r="C306" s="3"/>
       <c r="D306" s="3"/>
@@ -7882,7 +7883,7 @@
       <c r="I306" s="3"/>
     </row>
     <row r="307" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A307" s="11"/>
+      <c r="A307" s="9"/>
       <c r="B307" s="3"/>
       <c r="C307" s="3"/>
       <c r="D307" s="3"/>
@@ -7893,7 +7894,7 @@
       <c r="I307" s="3"/>
     </row>
     <row r="308" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A308" s="11"/>
+      <c r="A308" s="9"/>
       <c r="B308" s="3"/>
       <c r="C308" s="3"/>
       <c r="D308" s="3"/>
@@ -7904,7 +7905,7 @@
       <c r="I308" s="3"/>
     </row>
     <row r="309" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A309" s="11"/>
+      <c r="A309" s="9"/>
       <c r="B309" s="3"/>
       <c r="C309" s="3"/>
       <c r="D309" s="3"/>
@@ -7915,7 +7916,7 @@
       <c r="I309" s="3"/>
     </row>
     <row r="310" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A310" s="11"/>
+      <c r="A310" s="9"/>
       <c r="B310" s="3"/>
       <c r="C310" s="3"/>
       <c r="D310" s="3"/>
@@ -7926,7 +7927,7 @@
       <c r="I310" s="3"/>
     </row>
     <row r="311" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A311" s="11"/>
+      <c r="A311" s="9"/>
       <c r="B311" s="3"/>
       <c r="C311" s="3"/>
       <c r="D311" s="3"/>
@@ -7937,7 +7938,7 @@
       <c r="I311" s="3"/>
     </row>
     <row r="312" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A312" s="11"/>
+      <c r="A312" s="9"/>
       <c r="B312" s="3"/>
       <c r="C312" s="3"/>
       <c r="D312" s="3"/>
@@ -7948,7 +7949,7 @@
       <c r="I312" s="3"/>
     </row>
     <row r="313" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A313" s="11"/>
+      <c r="A313" s="9"/>
       <c r="B313" s="3"/>
       <c r="C313" s="3"/>
       <c r="D313" s="3"/>
@@ -7959,7 +7960,7 @@
       <c r="I313" s="3"/>
     </row>
     <row r="314" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A314" s="11"/>
+      <c r="A314" s="9"/>
       <c r="B314" s="3"/>
       <c r="C314" s="3"/>
       <c r="D314" s="3"/>
@@ -7970,7 +7971,7 @@
       <c r="I314" s="3"/>
     </row>
     <row r="315" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A315" s="11"/>
+      <c r="A315" s="9"/>
       <c r="B315" s="3"/>
       <c r="C315" s="3"/>
       <c r="D315" s="3"/>
@@ -7981,7 +7982,7 @@
       <c r="I315" s="3"/>
     </row>
     <row r="316" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A316" s="11"/>
+      <c r="A316" s="9"/>
       <c r="B316" s="3"/>
       <c r="C316" s="3"/>
       <c r="D316" s="3"/>
@@ -7992,7 +7993,7 @@
       <c r="I316" s="3"/>
     </row>
     <row r="317" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A317" s="11"/>
+      <c r="A317" s="9"/>
       <c r="B317" s="3"/>
       <c r="C317" s="3"/>
       <c r="D317" s="3"/>
@@ -8003,7 +8004,7 @@
       <c r="I317" s="3"/>
     </row>
     <row r="318" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A318" s="11"/>
+      <c r="A318" s="9"/>
       <c r="B318" s="3"/>
       <c r="C318" s="3"/>
       <c r="D318" s="3"/>
@@ -8014,7 +8015,7 @@
       <c r="I318" s="3"/>
     </row>
     <row r="319" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A319" s="11"/>
+      <c r="A319" s="9"/>
       <c r="B319" s="3"/>
       <c r="C319" s="3"/>
       <c r="D319" s="3"/>
@@ -8025,7 +8026,7 @@
       <c r="I319" s="3"/>
     </row>
     <row r="320" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A320" s="11"/>
+      <c r="A320" s="9"/>
       <c r="B320" s="3"/>
       <c r="C320" s="3"/>
       <c r="D320" s="3"/>
@@ -8036,7 +8037,7 @@
       <c r="I320" s="3"/>
     </row>
     <row r="321" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A321" s="11"/>
+      <c r="A321" s="9"/>
       <c r="B321" s="3"/>
       <c r="C321" s="3"/>
       <c r="D321" s="3"/>
@@ -8047,7 +8048,7 @@
       <c r="I321" s="3"/>
     </row>
     <row r="322" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A322" s="11"/>
+      <c r="A322" s="9"/>
       <c r="B322" s="3"/>
       <c r="C322" s="3"/>
       <c r="D322" s="3"/>
@@ -8058,7 +8059,7 @@
       <c r="I322" s="3"/>
     </row>
     <row r="323" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A323" s="11"/>
+      <c r="A323" s="9"/>
       <c r="B323" s="3"/>
       <c r="C323" s="3"/>
       <c r="D323" s="3"/>
@@ -8069,7 +8070,7 @@
       <c r="I323" s="3"/>
     </row>
     <row r="324" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A324" s="11"/>
+      <c r="A324" s="9"/>
       <c r="B324" s="3"/>
       <c r="C324" s="3"/>
       <c r="D324" s="3"/>
@@ -8080,7 +8081,7 @@
       <c r="I324" s="3"/>
     </row>
     <row r="325" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A325" s="11"/>
+      <c r="A325" s="9"/>
       <c r="B325" s="3"/>
       <c r="C325" s="3"/>
       <c r="D325" s="3"/>
@@ -8091,7 +8092,7 @@
       <c r="I325" s="3"/>
     </row>
     <row r="326" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A326" s="11"/>
+      <c r="A326" s="9"/>
       <c r="B326" s="3"/>
       <c r="C326" s="3"/>
       <c r="D326" s="3"/>
@@ -8102,7 +8103,7 @@
       <c r="I326" s="3"/>
     </row>
     <row r="327" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A327" s="11"/>
+      <c r="A327" s="9"/>
       <c r="B327" s="3"/>
       <c r="C327" s="3"/>
       <c r="D327" s="3"/>
@@ -8113,7 +8114,7 @@
       <c r="I327" s="3"/>
     </row>
     <row r="328" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A328" s="11"/>
+      <c r="A328" s="9"/>
       <c r="B328" s="3"/>
       <c r="C328" s="3"/>
       <c r="D328" s="3"/>
@@ -8124,7 +8125,7 @@
       <c r="I328" s="3"/>
     </row>
     <row r="329" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A329" s="11"/>
+      <c r="A329" s="9"/>
       <c r="B329" s="3"/>
       <c r="C329" s="3"/>
       <c r="D329" s="3"/>
@@ -8135,7 +8136,7 @@
       <c r="I329" s="3"/>
     </row>
     <row r="330" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A330" s="11"/>
+      <c r="A330" s="9"/>
       <c r="B330" s="3"/>
       <c r="C330" s="3"/>
       <c r="D330" s="3"/>
@@ -8146,7 +8147,7 @@
       <c r="I330" s="3"/>
     </row>
     <row r="331" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A331" s="11"/>
+      <c r="A331" s="9"/>
       <c r="B331" s="3"/>
       <c r="C331" s="3"/>
       <c r="D331" s="3"/>
@@ -8157,7 +8158,7 @@
       <c r="I331" s="3"/>
     </row>
     <row r="332" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A332" s="11"/>
+      <c r="A332" s="9"/>
       <c r="B332" s="3"/>
       <c r="C332" s="3"/>
       <c r="D332" s="3"/>
@@ -8168,7 +8169,7 @@
       <c r="I332" s="3"/>
     </row>
     <row r="333" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A333" s="11"/>
+      <c r="A333" s="9"/>
       <c r="B333" s="3"/>
       <c r="C333" s="3"/>
       <c r="D333" s="3"/>
@@ -8179,7 +8180,7 @@
       <c r="I333" s="3"/>
     </row>
     <row r="334" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A334" s="11"/>
+      <c r="A334" s="9"/>
       <c r="B334" s="3"/>
       <c r="C334" s="3"/>
       <c r="D334" s="3"/>
@@ -8190,7 +8191,7 @@
       <c r="I334" s="3"/>
     </row>
     <row r="335" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A335" s="11"/>
+      <c r="A335" s="9"/>
       <c r="B335" s="3"/>
       <c r="C335" s="3"/>
       <c r="D335" s="3"/>
@@ -8201,7 +8202,7 @@
       <c r="I335" s="3"/>
     </row>
     <row r="336" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A336" s="11"/>
+      <c r="A336" s="9"/>
       <c r="B336" s="3"/>
       <c r="C336" s="3"/>
       <c r="D336" s="3"/>
@@ -8212,7 +8213,7 @@
       <c r="I336" s="3"/>
     </row>
     <row r="337" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A337" s="11"/>
+      <c r="A337" s="9"/>
       <c r="B337" s="3"/>
       <c r="C337" s="3"/>
       <c r="D337" s="3"/>
@@ -8223,7 +8224,7 @@
       <c r="I337" s="3"/>
     </row>
     <row r="338" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A338" s="11"/>
+      <c r="A338" s="9"/>
       <c r="B338" s="3"/>
       <c r="C338" s="3"/>
       <c r="D338" s="3"/>
@@ -8234,7 +8235,7 @@
       <c r="I338" s="3"/>
     </row>
     <row r="339" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A339" s="11"/>
+      <c r="A339" s="9"/>
       <c r="B339" s="3"/>
       <c r="C339" s="3"/>
       <c r="D339" s="3"/>
@@ -8245,7 +8246,7 @@
       <c r="I339" s="3"/>
     </row>
     <row r="340" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A340" s="11"/>
+      <c r="A340" s="9"/>
       <c r="B340" s="3"/>
       <c r="C340" s="3"/>
       <c r="D340" s="3"/>
@@ -8256,7 +8257,7 @@
       <c r="I340" s="3"/>
     </row>
     <row r="341" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A341" s="11"/>
+      <c r="A341" s="9"/>
       <c r="B341" s="3"/>
       <c r="C341" s="3"/>
       <c r="D341" s="3"/>
@@ -8267,7 +8268,7 @@
       <c r="I341" s="3"/>
     </row>
     <row r="342" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A342" s="11"/>
+      <c r="A342" s="9"/>
       <c r="B342" s="3"/>
       <c r="C342" s="3"/>
       <c r="D342" s="3"/>
@@ -8278,7 +8279,7 @@
       <c r="I342" s="3"/>
     </row>
     <row r="343" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A343" s="11"/>
+      <c r="A343" s="9"/>
       <c r="B343" s="3"/>
       <c r="C343" s="3"/>
       <c r="D343" s="3"/>
@@ -8289,7 +8290,7 @@
       <c r="I343" s="3"/>
     </row>
     <row r="344" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A344" s="11"/>
+      <c r="A344" s="9"/>
       <c r="B344" s="3"/>
       <c r="C344" s="3"/>
       <c r="D344" s="3"/>
@@ -8300,7 +8301,7 @@
       <c r="I344" s="3"/>
     </row>
     <row r="345" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A345" s="11"/>
+      <c r="A345" s="9"/>
       <c r="B345" s="3"/>
       <c r="C345" s="3"/>
       <c r="D345" s="3"/>
@@ -8311,7 +8312,7 @@
       <c r="I345" s="3"/>
     </row>
     <row r="346" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A346" s="11"/>
+      <c r="A346" s="9"/>
       <c r="B346" s="3"/>
       <c r="C346" s="3"/>
       <c r="D346" s="3"/>
@@ -8322,7 +8323,7 @@
       <c r="I346" s="3"/>
     </row>
     <row r="347" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A347" s="11"/>
+      <c r="A347" s="9"/>
       <c r="B347" s="3"/>
       <c r="C347" s="3"/>
       <c r="D347" s="3"/>
@@ -8333,7 +8334,7 @@
       <c r="I347" s="3"/>
     </row>
     <row r="348" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A348" s="11"/>
+      <c r="A348" s="9"/>
       <c r="B348" s="3"/>
       <c r="C348" s="3"/>
       <c r="D348" s="3"/>
@@ -8344,7 +8345,7 @@
       <c r="I348" s="3"/>
     </row>
     <row r="349" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A349" s="11"/>
+      <c r="A349" s="9"/>
       <c r="B349" s="3"/>
       <c r="C349" s="3"/>
       <c r="D349" s="3"/>
@@ -8355,7 +8356,7 @@
       <c r="I349" s="3"/>
     </row>
     <row r="350" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A350" s="11"/>
+      <c r="A350" s="9"/>
       <c r="B350" s="3"/>
       <c r="C350" s="3"/>
       <c r="D350" s="3"/>
@@ -8366,7 +8367,7 @@
       <c r="I350" s="3"/>
     </row>
     <row r="351" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A351" s="11"/>
+      <c r="A351" s="9"/>
       <c r="B351" s="3"/>
       <c r="C351" s="3"/>
       <c r="D351" s="3"/>
@@ -8377,7 +8378,7 @@
       <c r="I351" s="3"/>
     </row>
     <row r="352" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A352" s="11"/>
+      <c r="A352" s="9"/>
       <c r="B352" s="3"/>
       <c r="C352" s="3"/>
       <c r="D352" s="3"/>
@@ -8388,7 +8389,7 @@
       <c r="I352" s="3"/>
     </row>
     <row r="353" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A353" s="11"/>
+      <c r="A353" s="9"/>
       <c r="B353" s="3"/>
       <c r="C353" s="3"/>
       <c r="D353" s="3"/>
@@ -8399,7 +8400,7 @@
       <c r="I353" s="3"/>
     </row>
     <row r="354" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A354" s="11"/>
+      <c r="A354" s="9"/>
       <c r="B354" s="3"/>
       <c r="C354" s="3"/>
       <c r="D354" s="3"/>
@@ -8410,7 +8411,7 @@
       <c r="I354" s="3"/>
     </row>
     <row r="355" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A355" s="11"/>
+      <c r="A355" s="9"/>
       <c r="B355" s="3"/>
       <c r="C355" s="3"/>
       <c r="D355" s="3"/>
@@ -8421,7 +8422,7 @@
       <c r="I355" s="3"/>
     </row>
     <row r="356" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A356" s="11"/>
+      <c r="A356" s="9"/>
       <c r="B356" s="3"/>
       <c r="C356" s="3"/>
       <c r="D356" s="3"/>
@@ -8432,7 +8433,7 @@
       <c r="I356" s="3"/>
     </row>
     <row r="357" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A357" s="11"/>
+      <c r="A357" s="9"/>
       <c r="B357" s="3"/>
       <c r="C357" s="3"/>
       <c r="D357" s="3"/>
@@ -8443,7 +8444,7 @@
       <c r="I357" s="3"/>
     </row>
     <row r="358" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A358" s="11"/>
+      <c r="A358" s="9"/>
       <c r="B358" s="3"/>
       <c r="C358" s="3"/>
       <c r="D358" s="3"/>
@@ -8454,7 +8455,7 @@
       <c r="I358" s="3"/>
     </row>
     <row r="359" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A359" s="11"/>
+      <c r="A359" s="9"/>
       <c r="B359" s="3"/>
       <c r="C359" s="3"/>
       <c r="D359" s="3"/>
@@ -8465,7 +8466,7 @@
       <c r="I359" s="3"/>
     </row>
     <row r="360" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A360" s="11"/>
+      <c r="A360" s="9"/>
       <c r="B360" s="3"/>
       <c r="C360" s="3"/>
       <c r="D360" s="3"/>
@@ -8476,7 +8477,7 @@
       <c r="I360" s="3"/>
     </row>
     <row r="361" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A361" s="11"/>
+      <c r="A361" s="9"/>
       <c r="B361" s="3"/>
       <c r="C361" s="3"/>
       <c r="D361" s="3"/>
@@ -8487,7 +8488,7 @@
       <c r="I361" s="3"/>
     </row>
     <row r="362" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A362" s="11"/>
+      <c r="A362" s="9"/>
       <c r="B362" s="3"/>
       <c r="C362" s="3"/>
       <c r="D362" s="3"/>
@@ -8498,7 +8499,7 @@
       <c r="I362" s="3"/>
     </row>
     <row r="363" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A363" s="11"/>
+      <c r="A363" s="9"/>
       <c r="B363" s="3"/>
       <c r="C363" s="3"/>
       <c r="D363" s="3"/>
@@ -8509,7 +8510,7 @@
       <c r="I363" s="3"/>
     </row>
     <row r="364" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A364" s="11"/>
+      <c r="A364" s="9"/>
       <c r="B364" s="3"/>
       <c r="C364" s="3"/>
       <c r="D364" s="3"/>
@@ -8520,7 +8521,7 @@
       <c r="I364" s="3"/>
     </row>
     <row r="365" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A365" s="11"/>
+      <c r="A365" s="9"/>
       <c r="B365" s="3"/>
       <c r="C365" s="3"/>
       <c r="D365" s="3"/>
@@ -8531,7 +8532,7 @@
       <c r="I365" s="3"/>
     </row>
     <row r="366" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A366" s="11"/>
+      <c r="A366" s="9"/>
       <c r="B366" s="3"/>
       <c r="C366" s="3"/>
       <c r="D366" s="3"/>
@@ -8542,7 +8543,7 @@
       <c r="I366" s="3"/>
     </row>
     <row r="367" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A367" s="11"/>
+      <c r="A367" s="9"/>
       <c r="B367" s="3"/>
       <c r="C367" s="3"/>
       <c r="D367" s="3"/>
@@ -8553,7 +8554,7 @@
       <c r="I367" s="3"/>
     </row>
     <row r="368" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A368" s="11"/>
+      <c r="A368" s="9"/>
       <c r="B368" s="3"/>
       <c r="C368" s="3"/>
       <c r="D368" s="3"/>
@@ -8564,7 +8565,7 @@
       <c r="I368" s="3"/>
     </row>
     <row r="369" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A369" s="11"/>
+      <c r="A369" s="9"/>
       <c r="B369" s="3"/>
       <c r="C369" s="3"/>
       <c r="D369" s="3"/>
@@ -8575,7 +8576,7 @@
       <c r="I369" s="3"/>
     </row>
     <row r="370" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A370" s="11"/>
+      <c r="A370" s="9"/>
       <c r="B370" s="3"/>
       <c r="C370" s="3"/>
       <c r="D370" s="3"/>
@@ -8586,7 +8587,7 @@
       <c r="I370" s="3"/>
     </row>
     <row r="371" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A371" s="11"/>
+      <c r="A371" s="9"/>
       <c r="B371" s="3"/>
       <c r="C371" s="3"/>
       <c r="D371" s="3"/>
@@ -8597,7 +8598,7 @@
       <c r="I371" s="3"/>
     </row>
     <row r="372" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A372" s="11"/>
+      <c r="A372" s="9"/>
       <c r="B372" s="3"/>
       <c r="C372" s="3"/>
       <c r="D372" s="3"/>
@@ -8608,7 +8609,7 @@
       <c r="I372" s="3"/>
     </row>
     <row r="373" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A373" s="11"/>
+      <c r="A373" s="9"/>
       <c r="B373" s="3"/>
       <c r="C373" s="3"/>
       <c r="D373" s="3"/>
@@ -8619,7 +8620,7 @@
       <c r="I373" s="3"/>
     </row>
     <row r="374" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A374" s="11"/>
+      <c r="A374" s="9"/>
       <c r="B374" s="3"/>
       <c r="C374" s="3"/>
       <c r="D374" s="3"/>
@@ -8630,7 +8631,7 @@
       <c r="I374" s="3"/>
     </row>
     <row r="375" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A375" s="11"/>
+      <c r="A375" s="9"/>
       <c r="B375" s="3"/>
       <c r="C375" s="3"/>
       <c r="D375" s="3"/>
@@ -8641,7 +8642,7 @@
       <c r="I375" s="3"/>
     </row>
     <row r="376" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A376" s="11"/>
+      <c r="A376" s="9"/>
       <c r="B376" s="3"/>
       <c r="C376" s="3"/>
       <c r="D376" s="3"/>
@@ -8652,7 +8653,7 @@
       <c r="I376" s="3"/>
     </row>
     <row r="377" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A377" s="11"/>
+      <c r="A377" s="9"/>
       <c r="B377" s="3"/>
       <c r="C377" s="3"/>
       <c r="D377" s="3"/>
@@ -8663,7 +8664,7 @@
       <c r="I377" s="3"/>
     </row>
     <row r="378" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A378" s="11"/>
+      <c r="A378" s="9"/>
       <c r="B378" s="3"/>
       <c r="C378" s="3"/>
       <c r="D378" s="3"/>
@@ -8674,7 +8675,7 @@
       <c r="I378" s="3"/>
     </row>
     <row r="379" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A379" s="11"/>
+      <c r="A379" s="9"/>
       <c r="B379" s="3"/>
       <c r="C379" s="3"/>
       <c r="D379" s="3"/>
@@ -8685,7 +8686,7 @@
       <c r="I379" s="3"/>
     </row>
     <row r="380" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A380" s="11"/>
+      <c r="A380" s="9"/>
       <c r="B380" s="3"/>
       <c r="C380" s="3"/>
       <c r="D380" s="3"/>
@@ -8696,7 +8697,7 @@
       <c r="I380" s="3"/>
     </row>
     <row r="381" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A381" s="11"/>
+      <c r="A381" s="9"/>
       <c r="B381" s="3"/>
       <c r="C381" s="3"/>
       <c r="D381" s="3"/>
@@ -8707,7 +8708,7 @@
       <c r="I381" s="3"/>
     </row>
     <row r="382" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A382" s="11"/>
+      <c r="A382" s="9"/>
       <c r="B382" s="3"/>
       <c r="C382" s="3"/>
       <c r="D382" s="3"/>
@@ -8718,7 +8719,7 @@
       <c r="I382" s="3"/>
     </row>
     <row r="383" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A383" s="11"/>
+      <c r="A383" s="9"/>
       <c r="B383" s="3"/>
       <c r="C383" s="3"/>
       <c r="D383" s="3"/>
@@ -8729,7 +8730,7 @@
       <c r="I383" s="3"/>
     </row>
     <row r="384" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A384" s="11"/>
+      <c r="A384" s="9"/>
       <c r="B384" s="3"/>
       <c r="C384" s="3"/>
       <c r="D384" s="3"/>
@@ -8740,7 +8741,7 @@
       <c r="I384" s="3"/>
     </row>
     <row r="385" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A385" s="11"/>
+      <c r="A385" s="9"/>
       <c r="B385" s="3"/>
       <c r="C385" s="3"/>
       <c r="D385" s="3"/>
@@ -8751,7 +8752,7 @@
       <c r="I385" s="3"/>
     </row>
     <row r="386" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A386" s="11"/>
+      <c r="A386" s="9"/>
       <c r="B386" s="3"/>
       <c r="C386" s="3"/>
       <c r="D386" s="3"/>
@@ -8762,7 +8763,7 @@
       <c r="I386" s="3"/>
     </row>
     <row r="387" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A387" s="11"/>
+      <c r="A387" s="9"/>
       <c r="B387" s="3"/>
       <c r="C387" s="3"/>
       <c r="D387" s="3"/>
@@ -8773,7 +8774,7 @@
       <c r="I387" s="3"/>
     </row>
     <row r="388" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A388" s="11"/>
+      <c r="A388" s="9"/>
       <c r="B388" s="3"/>
       <c r="C388" s="3"/>
       <c r="D388" s="3"/>
@@ -8784,7 +8785,7 @@
       <c r="I388" s="3"/>
     </row>
     <row r="389" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A389" s="11"/>
+      <c r="A389" s="9"/>
       <c r="B389" s="3"/>
       <c r="C389" s="3"/>
       <c r="D389" s="3"/>
@@ -8795,7 +8796,7 @@
       <c r="I389" s="3"/>
     </row>
     <row r="390" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A390" s="11"/>
+      <c r="A390" s="9"/>
       <c r="B390" s="3"/>
       <c r="C390" s="3"/>
       <c r="D390" s="3"/>
@@ -8806,7 +8807,7 @@
       <c r="I390" s="3"/>
     </row>
     <row r="391" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A391" s="11"/>
+      <c r="A391" s="9"/>
       <c r="B391" s="3"/>
       <c r="C391" s="3"/>
       <c r="D391" s="3"/>
@@ -8817,7 +8818,7 @@
       <c r="I391" s="3"/>
     </row>
     <row r="392" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A392" s="11"/>
+      <c r="A392" s="9"/>
       <c r="B392" s="3"/>
       <c r="C392" s="3"/>
       <c r="D392" s="3"/>
@@ -8828,7 +8829,7 @@
       <c r="I392" s="3"/>
     </row>
     <row r="393" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A393" s="11"/>
+      <c r="A393" s="9"/>
       <c r="B393" s="3"/>
       <c r="C393" s="3"/>
       <c r="D393" s="3"/>
@@ -8839,7 +8840,7 @@
       <c r="I393" s="3"/>
     </row>
     <row r="394" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A394" s="11"/>
+      <c r="A394" s="9"/>
       <c r="B394" s="3"/>
       <c r="C394" s="3"/>
       <c r="D394" s="3"/>
@@ -8850,7 +8851,7 @@
       <c r="I394" s="3"/>
     </row>
     <row r="395" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A395" s="11"/>
+      <c r="A395" s="9"/>
       <c r="B395" s="3"/>
       <c r="C395" s="3"/>
       <c r="D395" s="3"/>
@@ -8861,7 +8862,7 @@
       <c r="I395" s="3"/>
     </row>
     <row r="396" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A396" s="11"/>
+      <c r="A396" s="9"/>
       <c r="B396" s="3"/>
       <c r="C396" s="3"/>
       <c r="D396" s="3"/>
@@ -8872,7 +8873,7 @@
       <c r="I396" s="3"/>
     </row>
     <row r="397" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A397" s="11"/>
+      <c r="A397" s="9"/>
       <c r="B397" s="3"/>
       <c r="C397" s="3"/>
       <c r="D397" s="3"/>
@@ -8883,7 +8884,7 @@
       <c r="I397" s="3"/>
     </row>
     <row r="398" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A398" s="11"/>
+      <c r="A398" s="9"/>
       <c r="B398" s="3"/>
       <c r="C398" s="3"/>
       <c r="D398" s="3"/>
@@ -8894,7 +8895,7 @@
       <c r="I398" s="3"/>
     </row>
     <row r="399" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A399" s="11"/>
+      <c r="A399" s="9"/>
       <c r="B399" s="3"/>
       <c r="C399" s="3"/>
       <c r="D399" s="3"/>
@@ -8905,7 +8906,7 @@
       <c r="I399" s="3"/>
     </row>
     <row r="400" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A400" s="11"/>
+      <c r="A400" s="9"/>
       <c r="B400" s="3"/>
       <c r="C400" s="3"/>
       <c r="D400" s="3"/>
@@ -8916,7 +8917,7 @@
       <c r="I400" s="3"/>
     </row>
     <row r="401" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A401" s="11"/>
+      <c r="A401" s="9"/>
       <c r="B401" s="3"/>
       <c r="C401" s="3"/>
       <c r="D401" s="3"/>
@@ -8927,7 +8928,7 @@
       <c r="I401" s="3"/>
     </row>
     <row r="402" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A402" s="11"/>
+      <c r="A402" s="9"/>
       <c r="B402" s="3"/>
       <c r="C402" s="3"/>
       <c r="D402" s="3"/>
@@ -8938,7 +8939,7 @@
       <c r="I402" s="3"/>
     </row>
     <row r="403" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A403" s="11"/>
+      <c r="A403" s="9"/>
       <c r="B403" s="3"/>
       <c r="C403" s="3"/>
       <c r="D403" s="3"/>
@@ -8949,7 +8950,7 @@
       <c r="I403" s="3"/>
     </row>
     <row r="404" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A404" s="11"/>
+      <c r="A404" s="9"/>
       <c r="B404" s="3"/>
       <c r="C404" s="3"/>
       <c r="D404" s="3"/>
@@ -8960,7 +8961,7 @@
       <c r="I404" s="3"/>
     </row>
     <row r="405" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A405" s="11"/>
+      <c r="A405" s="9"/>
       <c r="B405" s="3"/>
       <c r="C405" s="3"/>
       <c r="D405" s="3"/>
@@ -8971,7 +8972,7 @@
       <c r="I405" s="3"/>
     </row>
     <row r="406" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A406" s="11"/>
+      <c r="A406" s="9"/>
       <c r="B406" s="3"/>
       <c r="C406" s="3"/>
       <c r="D406" s="3"/>
@@ -8982,7 +8983,7 @@
       <c r="I406" s="3"/>
     </row>
     <row r="407" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A407" s="11"/>
+      <c r="A407" s="9"/>
       <c r="B407" s="3"/>
       <c r="C407" s="3"/>
       <c r="D407" s="3"/>

</xml_diff>